<commit_message>
Ajout de nouveaux pokemon dans le fichier Excel Ajout des cartes énergies dans les images
</commit_message>
<xml_diff>
--- a/database/database.xlsx
+++ b/database/database.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\prj_perso\Cartes\project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\prj_perso\Cartes\project\CardsGame\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="259">
   <si>
     <t>Nom</t>
   </si>
@@ -760,6 +760,48 @@
   </si>
   <si>
     <t>Water</t>
+  </si>
+  <si>
+    <t>Lancez une pièce. Si c'est face, le Pokémon Défenseur est maintenant Empoisonné</t>
+  </si>
+  <si>
+    <t>Dard-venin</t>
+  </si>
+  <si>
+    <t>Lancez une pièce. Si c'est face, le Pokémon Défenseur est maintenant Confus.</t>
+  </si>
+  <si>
+    <t>Charge</t>
+  </si>
+  <si>
+    <t>Etreinte</t>
+  </si>
+  <si>
+    <t>Lancez une pièce. Si c'est face, le Pokémon défenseur est maintenant Paralysé.</t>
+  </si>
+  <si>
+    <t>Le Pokémon défenseur est maintenant Empoisonné.</t>
+  </si>
+  <si>
+    <t>Gifle</t>
+  </si>
+  <si>
+    <t>Soin</t>
+  </si>
+  <si>
+    <t>Défaussez une carte Énergie eau attachée à Staross pour pouvoir utiliser cette attaque. Retirez tous les marqueurs de dégâts sur Staross.</t>
+  </si>
+  <si>
+    <t>XX</t>
+  </si>
+  <si>
+    <t>Etoile gelante</t>
+  </si>
+  <si>
+    <t>Ruade</t>
+  </si>
+  <si>
+    <t>Queue de flamme</t>
   </si>
 </sst>
 </file>
@@ -1200,14 +1242,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:BR204"/>
+  <dimension ref="B1:BR204"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A149" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A82" sqref="A82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="2.42578125" customWidth="1"/>
     <col min="3" max="3" width="15.42578125" customWidth="1"/>
     <col min="9" max="9" width="12.85546875" customWidth="1"/>
     <col min="10" max="10" width="14.7109375" customWidth="1"/>
@@ -1219,6 +1263,7 @@
     <col min="32" max="32" width="78.5703125" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:69" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:69" x14ac:dyDescent="0.25">
       <c r="B2" s="10" t="s">
         <v>14</v>
@@ -2771,16 +2816,32 @@
       <c r="C17" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
+      <c r="D17" s="1">
+        <v>40</v>
+      </c>
+      <c r="E17" s="1">
+        <v>8</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0</v>
+      </c>
+      <c r="G17" s="1">
+        <v>5</v>
+      </c>
       <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
+      <c r="I17" s="1">
+        <v>1</v>
+      </c>
       <c r="J17" s="4"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
+      <c r="K17" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="M17" s="1">
+        <v>10</v>
+      </c>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
@@ -2789,15 +2850,21 @@
       <c r="S17" s="1"/>
       <c r="T17" s="1"/>
       <c r="U17" s="1"/>
-      <c r="V17" s="1"/>
+      <c r="V17" s="1">
+        <v>1</v>
+      </c>
       <c r="W17" s="1"/>
       <c r="X17" s="1"/>
       <c r="Y17" s="1"/>
       <c r="Z17" s="1"/>
       <c r="AA17" s="1"/>
       <c r="AB17" s="1"/>
-      <c r="AC17" s="1"/>
-      <c r="AD17" s="7"/>
+      <c r="AC17" s="1">
+        <v>2</v>
+      </c>
+      <c r="AD17" s="7">
+        <v>2</v>
+      </c>
       <c r="AE17" s="5"/>
       <c r="AF17" s="5"/>
       <c r="AG17" s="1"/>
@@ -4603,22 +4670,38 @@
       <c r="C41" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
+      <c r="D41" s="1">
+        <v>50</v>
+      </c>
+      <c r="E41" s="1">
+        <v>5</v>
+      </c>
       <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
+      <c r="G41" s="1">
+        <v>14</v>
+      </c>
       <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
+      <c r="I41" s="1">
+        <v>1</v>
+      </c>
       <c r="J41" s="4"/>
-      <c r="K41" s="6"/>
-      <c r="L41" s="1"/>
-      <c r="M41" s="1"/>
+      <c r="K41" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="L41" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="M41" s="1">
+        <v>10</v>
+      </c>
       <c r="N41" s="1"/>
       <c r="O41" s="1"/>
       <c r="P41" s="1"/>
       <c r="Q41" s="1"/>
       <c r="R41" s="1"/>
-      <c r="S41" s="1"/>
+      <c r="S41" s="1">
+        <v>2</v>
+      </c>
       <c r="T41" s="1"/>
       <c r="U41" s="1"/>
       <c r="V41" s="1"/>
@@ -4628,8 +4711,12 @@
       <c r="Z41" s="1"/>
       <c r="AA41" s="1"/>
       <c r="AB41" s="1"/>
-      <c r="AC41" s="1"/>
-      <c r="AD41" s="7"/>
+      <c r="AC41" s="1">
+        <v>2</v>
+      </c>
+      <c r="AD41" s="7">
+        <v>0</v>
+      </c>
       <c r="AE41" s="5"/>
       <c r="AF41" s="5"/>
       <c r="AG41" s="1"/>
@@ -7629,16 +7716,28 @@
       <c r="C81" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="D81" s="1"/>
-      <c r="E81" s="1"/>
+      <c r="D81" s="1">
+        <v>40</v>
+      </c>
+      <c r="E81" s="1">
+        <v>5</v>
+      </c>
       <c r="F81" s="1"/>
-      <c r="G81" s="1"/>
+      <c r="G81" s="1">
+        <v>14</v>
+      </c>
       <c r="H81" s="1"/>
-      <c r="I81" s="1"/>
+      <c r="I81" s="1">
+        <v>1</v>
+      </c>
       <c r="J81" s="4"/>
-      <c r="K81" s="6"/>
+      <c r="K81" s="6" t="s">
+        <v>257</v>
+      </c>
       <c r="L81" s="1"/>
-      <c r="M81" s="1"/>
+      <c r="M81" s="1">
+        <v>20</v>
+      </c>
       <c r="N81" s="1"/>
       <c r="O81" s="1"/>
       <c r="P81" s="1"/>
@@ -7649,22 +7748,30 @@
       <c r="U81" s="1"/>
       <c r="V81" s="1"/>
       <c r="W81" s="1"/>
-      <c r="X81" s="1"/>
+      <c r="X81" s="1">
+        <v>2</v>
+      </c>
       <c r="Y81" s="1"/>
       <c r="Z81" s="1"/>
       <c r="AA81" s="1"/>
       <c r="AB81" s="1"/>
       <c r="AC81" s="1"/>
       <c r="AD81" s="7"/>
-      <c r="AE81" s="5"/>
+      <c r="AE81" s="5" t="s">
+        <v>258</v>
+      </c>
       <c r="AF81" s="5"/>
-      <c r="AG81" s="1"/>
+      <c r="AG81" s="1">
+        <v>30</v>
+      </c>
       <c r="AH81" s="1"/>
       <c r="AI81" s="1"/>
       <c r="AJ81" s="1"/>
       <c r="AK81" s="1"/>
       <c r="AL81" s="1"/>
-      <c r="AM81" s="1"/>
+      <c r="AM81" s="1">
+        <v>2</v>
+      </c>
       <c r="AN81" s="1"/>
       <c r="AO81" s="1"/>
       <c r="AP81" s="1"/>
@@ -9353,16 +9460,28 @@
       <c r="C104" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="D104" s="1"/>
-      <c r="E104" s="1"/>
+      <c r="D104" s="1">
+        <v>40</v>
+      </c>
+      <c r="E104" s="1">
+        <v>3</v>
+      </c>
       <c r="F104" s="1"/>
-      <c r="G104" s="1"/>
+      <c r="G104" s="1">
+        <v>4</v>
+      </c>
       <c r="H104" s="1"/>
-      <c r="I104" s="1"/>
+      <c r="I104" s="1">
+        <v>1</v>
+      </c>
       <c r="J104" s="4"/>
-      <c r="K104" s="6"/>
+      <c r="K104" s="6" t="s">
+        <v>248</v>
+      </c>
       <c r="L104" s="1"/>
-      <c r="M104" s="1"/>
+      <c r="M104" s="1">
+        <v>10</v>
+      </c>
       <c r="N104" s="1"/>
       <c r="O104" s="1"/>
       <c r="P104" s="1"/>
@@ -9373,7 +9492,9 @@
       <c r="U104" s="1"/>
       <c r="V104" s="1"/>
       <c r="W104" s="1"/>
-      <c r="X104" s="1"/>
+      <c r="X104" s="1">
+        <v>1</v>
+      </c>
       <c r="Y104" s="1"/>
       <c r="Z104" s="1"/>
       <c r="AA104" s="1"/>
@@ -10399,16 +10520,30 @@
       <c r="C118" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="D118" s="1"/>
-      <c r="E118" s="1"/>
+      <c r="D118" s="1">
+        <v>50</v>
+      </c>
+      <c r="E118" s="1">
+        <v>8</v>
+      </c>
       <c r="F118" s="1"/>
-      <c r="G118" s="1"/>
+      <c r="G118" s="1">
+        <v>5</v>
+      </c>
       <c r="H118" s="1"/>
-      <c r="I118" s="1"/>
+      <c r="I118" s="1">
+        <v>2</v>
+      </c>
       <c r="J118" s="4"/>
-      <c r="K118" s="6"/>
-      <c r="L118" s="1"/>
-      <c r="M118" s="1"/>
+      <c r="K118" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="L118" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="M118" s="1">
+        <v>20</v>
+      </c>
       <c r="N118" s="1"/>
       <c r="O118" s="1"/>
       <c r="P118" s="1"/>
@@ -10417,18 +10552,32 @@
       <c r="S118" s="1"/>
       <c r="T118" s="1"/>
       <c r="U118" s="1"/>
-      <c r="V118" s="1"/>
+      <c r="V118" s="1">
+        <v>1</v>
+      </c>
       <c r="W118" s="1"/>
-      <c r="X118" s="1"/>
+      <c r="X118" s="1">
+        <v>1</v>
+      </c>
       <c r="Y118" s="1"/>
       <c r="Z118" s="1"/>
       <c r="AA118" s="1"/>
       <c r="AB118" s="1"/>
-      <c r="AC118" s="1"/>
-      <c r="AD118" s="7"/>
-      <c r="AE118" s="5"/>
-      <c r="AF118" s="5"/>
-      <c r="AG118" s="1"/>
+      <c r="AC118" s="1">
+        <v>2</v>
+      </c>
+      <c r="AD118" s="7">
+        <v>2</v>
+      </c>
+      <c r="AE118" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="AF118" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="AG118" s="1">
+        <v>20</v>
+      </c>
       <c r="AH118" s="1"/>
       <c r="AI118" s="1"/>
       <c r="AJ118" s="1"/>
@@ -10437,15 +10586,21 @@
       <c r="AM118" s="1"/>
       <c r="AN118" s="1"/>
       <c r="AO118" s="1"/>
-      <c r="AP118" s="1"/>
+      <c r="AP118" s="1">
+        <v>3</v>
+      </c>
       <c r="AQ118" s="1"/>
       <c r="AR118" s="1"/>
       <c r="AS118" s="1"/>
       <c r="AT118" s="1"/>
       <c r="AU118" s="1"/>
       <c r="AV118" s="1"/>
-      <c r="AW118" s="1"/>
-      <c r="AX118" s="4"/>
+      <c r="AW118" s="1">
+        <v>1</v>
+      </c>
+      <c r="AX118" s="4">
+        <v>3</v>
+      </c>
       <c r="AY118" s="6"/>
       <c r="AZ118" s="1"/>
       <c r="BA118" s="1"/>
@@ -10847,16 +11002,28 @@
       <c r="C124" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="D124" s="1"/>
-      <c r="E124" s="1"/>
+      <c r="D124" s="1">
+        <v>40</v>
+      </c>
+      <c r="E124" s="1">
+        <v>14</v>
+      </c>
       <c r="F124" s="1"/>
-      <c r="G124" s="1"/>
+      <c r="G124" s="1">
+        <v>3</v>
+      </c>
       <c r="H124" s="1"/>
-      <c r="I124" s="1"/>
+      <c r="I124" s="1">
+        <v>1</v>
+      </c>
       <c r="J124" s="4"/>
-      <c r="K124" s="6"/>
+      <c r="K124" s="6" t="s">
+        <v>252</v>
+      </c>
       <c r="L124" s="1"/>
-      <c r="M124" s="1"/>
+      <c r="M124" s="1">
+        <v>20</v>
+      </c>
       <c r="N124" s="1"/>
       <c r="O124" s="1"/>
       <c r="P124" s="1"/>
@@ -10871,7 +11038,9 @@
       <c r="Y124" s="1"/>
       <c r="Z124" s="1"/>
       <c r="AA124" s="1"/>
-      <c r="AB124" s="1"/>
+      <c r="AB124" s="1">
+        <v>1</v>
+      </c>
       <c r="AC124" s="1"/>
       <c r="AD124" s="7"/>
       <c r="AE124" s="5"/>
@@ -10921,18 +11090,32 @@
       <c r="C125" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="D125" s="1"/>
-      <c r="E125" s="1"/>
+      <c r="D125" s="1">
+        <v>60</v>
+      </c>
+      <c r="E125" s="1">
+        <v>14</v>
+      </c>
       <c r="F125" s="1"/>
-      <c r="G125" s="1"/>
+      <c r="G125" s="1">
+        <v>3</v>
+      </c>
       <c r="H125" s="1"/>
-      <c r="I125" s="1"/>
+      <c r="I125" s="1">
+        <v>1</v>
+      </c>
       <c r="J125" s="4">
         <v>120</v>
       </c>
-      <c r="K125" s="6"/>
-      <c r="L125" s="1"/>
-      <c r="M125" s="1"/>
+      <c r="K125" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="L125" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="M125" s="1">
+        <v>0</v>
+      </c>
       <c r="N125" s="1"/>
       <c r="O125" s="1"/>
       <c r="P125" s="1"/>
@@ -10947,12 +11130,24 @@
       <c r="Y125" s="1"/>
       <c r="Z125" s="1"/>
       <c r="AA125" s="1"/>
-      <c r="AB125" s="1"/>
-      <c r="AC125" s="1"/>
-      <c r="AD125" s="7"/>
-      <c r="AE125" s="5"/>
-      <c r="AF125" s="5"/>
-      <c r="AG125" s="1"/>
+      <c r="AB125" s="1">
+        <v>2</v>
+      </c>
+      <c r="AC125" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="AD125" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="AE125" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="AF125" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="AG125" s="1">
+        <v>20</v>
+      </c>
       <c r="AH125" s="1"/>
       <c r="AI125" s="1"/>
       <c r="AJ125" s="1"/>
@@ -10963,13 +11158,21 @@
       <c r="AO125" s="1"/>
       <c r="AP125" s="1"/>
       <c r="AQ125" s="1"/>
-      <c r="AR125" s="1"/>
+      <c r="AR125" s="1">
+        <v>2</v>
+      </c>
       <c r="AS125" s="1"/>
       <c r="AT125" s="1"/>
       <c r="AU125" s="1"/>
-      <c r="AV125" s="1"/>
-      <c r="AW125" s="1"/>
-      <c r="AX125" s="4"/>
+      <c r="AV125" s="1">
+        <v>1</v>
+      </c>
+      <c r="AW125" s="1">
+        <v>2</v>
+      </c>
+      <c r="AX125" s="4">
+        <v>2</v>
+      </c>
       <c r="AY125" s="6"/>
       <c r="AZ125" s="1"/>
       <c r="BA125" s="1"/>
@@ -16856,7 +17059,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>

</xml_diff>